<commit_message>
Fix Excel test case for Open Menu issue
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testdata.xlsx
+++ b/cypress/fixtures/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cypress\CypressAutomation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD75F9C3-0A21-4CE3-B5C1-15D5C6C87BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A22CF07-8587-4290-9D5A-3D90829FC48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{28FADA2D-E3F9-4A07-A0C4-1F4D7FE69298}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>standard_user</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>passg</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -416,7 +413,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,12 +455,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>